<commit_message>
Update techinical documentation for errors and WS
</commit_message>
<xml_diff>
--- a/docs/_static/xlsx/tab_Cessazione_unione_civile___convivenze.xlsx
+++ b/docs/_static/xlsx/tab_Cessazione_unione_civile___convivenze.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -43,19 +43,16 @@
     <t>Matrimonio</t>
   </si>
   <si>
-    <t>Decesso unito civilmente</t>
-  </si>
-  <si>
     <t>Accordo tra le parti</t>
   </si>
   <si>
     <t>Recesso unilaterale</t>
   </si>
   <si>
-    <t>Decesso convivente di fatto</t>
-  </si>
-  <si>
     <t>Matrimonio/unione civile</t>
+  </si>
+  <si>
+    <t>Decesso del convivente/unito civilmente</t>
   </si>
 </sst>
 </file>
@@ -403,17 +400,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625"/>
-    <col min="2" max="2" width="33.83203125"/>
+    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625"/>
     <col min="4" max="4" width="17.1640625"/>
     <col min="5" max="5" width="16"/>
@@ -470,7 +467,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -478,7 +475,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -486,7 +483,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -494,22 +491,15 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -646,13 +636,13 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3958BE9-611C-4D19-857D-1F92BB9E65A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>